<commit_message>
Update README and Analysis file
</commit_message>
<xml_diff>
--- a/Analysis/Statistical_errors.xlsx
+++ b/Analysis/Statistical_errors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,52 +436,52 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>wB97M2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>wB97M-V</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>CF22D</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>wB97X-V</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>revDSD-PBEP86-D4</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>M052X</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>M062X</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>M052X</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>M08HX</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>MN15</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>DSD-PBEPBE</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>r2SCAN0</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>MGGA_MS2h</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -522,52 +522,52 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.077233047728079</v>
+        <v>0.9485324850586064</v>
       </c>
       <c r="C2" t="n">
-        <v>1.250068438130513</v>
+        <v>1.075538502341131</v>
       </c>
       <c r="D2" t="n">
-        <v>1.320289764204146</v>
+        <v>1.24925710505858</v>
       </c>
       <c r="E2" t="n">
-        <v>1.96425214950025</v>
+        <v>1.312905121447046</v>
       </c>
       <c r="F2" t="n">
-        <v>1.970389385729717</v>
+        <v>1.521959467035516</v>
       </c>
       <c r="G2" t="n">
-        <v>1.990949781955851</v>
+        <v>1.941493346062861</v>
       </c>
       <c r="H2" t="n">
-        <v>2.022127722903106</v>
+        <v>1.971004445883499</v>
       </c>
       <c r="I2" t="n">
-        <v>2.109830400438947</v>
+        <v>1.993475061921084</v>
       </c>
       <c r="J2" t="n">
-        <v>2.801100060371369</v>
+        <v>2.009869356372007</v>
       </c>
       <c r="K2" t="n">
-        <v>3.265082909480225</v>
+        <v>2.811673997298874</v>
       </c>
       <c r="L2" t="n">
-        <v>3.315946817553699</v>
+        <v>3.277356932074</v>
       </c>
       <c r="M2" t="n">
-        <v>3.475533592492577</v>
+        <v>3.477682270471748</v>
       </c>
       <c r="N2" t="n">
-        <v>3.644627382331717</v>
+        <v>3.64800509733057</v>
       </c>
       <c r="O2" t="n">
-        <v>4.055507206538667</v>
+        <v>4.114856776341658</v>
       </c>
       <c r="P2" t="n">
-        <v>4.39897885004557</v>
+        <v>4.523620098569826</v>
       </c>
       <c r="Q2" t="n">
-        <v>5.664712104156976</v>
+        <v>5.691160285540097</v>
       </c>
     </row>
     <row r="3">
@@ -577,52 +577,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.061577773524401</v>
+        <v>0.6682301509999483</v>
       </c>
       <c r="C3" t="n">
-        <v>1.117046689098634</v>
+        <v>1.061577794867771</v>
       </c>
       <c r="D3" t="n">
-        <v>1.567957967488491</v>
+        <v>1.117046707592176</v>
       </c>
       <c r="E3" t="n">
-        <v>1.538446086223357</v>
+        <v>1.567957998053436</v>
       </c>
       <c r="F3" t="n">
-        <v>1.980175150255925</v>
+        <v>1.216549573109172</v>
       </c>
       <c r="G3" t="n">
-        <v>1.253832167672462</v>
+        <v>1.980175216602123</v>
       </c>
       <c r="H3" t="n">
-        <v>1.367874864363381</v>
+        <v>1.538446146087755</v>
       </c>
       <c r="I3" t="n">
-        <v>1.037873678314696</v>
+        <v>1.253832196919273</v>
       </c>
       <c r="J3" t="n">
-        <v>2.075873035792043</v>
+        <v>1.367874893291673</v>
       </c>
       <c r="K3" t="n">
-        <v>2.317207845517341</v>
+        <v>2.075873118633174</v>
       </c>
       <c r="L3" t="n">
-        <v>1.93930005327659</v>
+        <v>1.939300075785767</v>
       </c>
       <c r="M3" t="n">
-        <v>2.430498326109255</v>
+        <v>2.43049842142372</v>
       </c>
       <c r="N3" t="n">
-        <v>2.261613544989141</v>
+        <v>2.261613590144001</v>
       </c>
       <c r="O3" t="n">
-        <v>1.538501416177459</v>
+        <v>1.538501449436001</v>
       </c>
       <c r="P3" t="n">
-        <v>1.631565348070078</v>
+        <v>1.631565374781163</v>
       </c>
       <c r="Q3" t="n">
-        <v>3.292905217482136</v>
+        <v>3.292905240210722</v>
       </c>
     </row>
     <row r="4">
@@ -632,52 +632,52 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.807239366393285</v>
+        <v>1.03890582617713</v>
       </c>
       <c r="C4" t="n">
-        <v>1.981623492630044</v>
+        <v>1.807239366370509</v>
       </c>
       <c r="D4" t="n">
-        <v>1.040893097789385</v>
+        <v>1.981623492615641</v>
       </c>
       <c r="E4" t="n">
-        <v>1.020916802390297</v>
+        <v>1.040893097767846</v>
       </c>
       <c r="F4" t="n">
-        <v>1.062329342682693</v>
+        <v>1.887403100208598</v>
       </c>
       <c r="G4" t="n">
-        <v>1.205935272134945</v>
+        <v>1.062329342658534</v>
       </c>
       <c r="H4" t="n">
-        <v>1.537183742212589</v>
+        <v>1.020916802364601</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8940627876449463</v>
+        <v>1.205935272086035</v>
       </c>
       <c r="J4" t="n">
-        <v>1.116138938895665</v>
+        <v>1.53718374217268</v>
       </c>
       <c r="K4" t="n">
-        <v>1.643826963035098</v>
+        <v>1.116138939705384</v>
       </c>
       <c r="L4" t="n">
-        <v>1.472469255888884</v>
+        <v>1.472469255840157</v>
       </c>
       <c r="M4" t="n">
-        <v>1.568537354187785</v>
+        <v>1.568537354139071</v>
       </c>
       <c r="N4" t="n">
-        <v>1.298727770634585</v>
+        <v>1.298727770613418</v>
       </c>
       <c r="O4" t="n">
-        <v>1.089285966467236</v>
+        <v>1.089285966430315</v>
       </c>
       <c r="P4" t="n">
-        <v>1.045057997701087</v>
+        <v>1.045057997675376</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.068887455726755</v>
+        <v>2.068887455683881</v>
       </c>
     </row>
     <row r="5">
@@ -687,272 +687,327 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9247261664342316</v>
+        <v>0.8761390189112278</v>
       </c>
       <c r="C5" t="n">
-        <v>2.860531380880627</v>
+        <v>0.9247261666421355</v>
       </c>
       <c r="D5" t="n">
-        <v>1.190705328572716</v>
+        <v>2.860531381523753</v>
       </c>
       <c r="E5" t="n">
-        <v>1.013570648489794</v>
+        <v>1.190705328840419</v>
       </c>
       <c r="F5" t="n">
-        <v>1.322852217050168</v>
+        <v>0.3264042308092379</v>
       </c>
       <c r="G5" t="n">
-        <v>1.251333003068837</v>
+        <v>1.322852217347581</v>
       </c>
       <c r="H5" t="n">
-        <v>1.762850697671111</v>
+        <v>1.013570648717671</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6835104635424711</v>
+        <v>1.25133300335017</v>
       </c>
       <c r="J5" t="n">
-        <v>1.666019384378192</v>
+        <v>1.762850698067449</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9154032304374173</v>
+        <v>1.666020535376949</v>
       </c>
       <c r="L5" t="n">
-        <v>1.45563382236109</v>
+        <v>1.455633822688355</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7235033583110502</v>
+        <v>0.7235033584737127</v>
       </c>
       <c r="N5" t="n">
-        <v>1.062130677600046</v>
+        <v>1.062130677838842</v>
       </c>
       <c r="O5" t="n">
-        <v>1.362824441810818</v>
+        <v>1.362824442117218</v>
       </c>
       <c r="P5" t="n">
-        <v>1.099713276974023</v>
+        <v>1.099713284993532</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.060830648438262</v>
+        <v>1.060830648676765</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Mean Isomerization</t>
+          <t>Mean Intramolecular Noncovalent</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.088030198686702</v>
+        <v>1.021274463647786</v>
       </c>
       <c r="C6" t="n">
-        <v>1.204269820286066</v>
+        <v>1.070760594234186</v>
       </c>
       <c r="D6" t="n">
-        <v>1.363310819753531</v>
+        <v>1.254228493669825</v>
       </c>
       <c r="E6" t="n">
-        <v>2.26388136325991</v>
+        <v>0.9298746049867764</v>
       </c>
       <c r="F6" t="n">
-        <v>1.713167289503553</v>
+        <v>1.003151392433528</v>
       </c>
       <c r="G6" t="n">
-        <v>2.485952100463995</v>
+        <v>1.707520689303506</v>
       </c>
       <c r="H6" t="n">
-        <v>2.821451592428313</v>
+        <v>1.974323386417983</v>
       </c>
       <c r="I6" t="n">
-        <v>2.49730206935181</v>
+        <v>2.964708231009484</v>
       </c>
       <c r="J6" t="n">
-        <v>2.990280481040097</v>
+        <v>3.71778634826125</v>
       </c>
       <c r="K6" t="n">
-        <v>3.549324430881538</v>
+        <v>3.425001568048197</v>
       </c>
       <c r="L6" t="n">
-        <v>3.488845576381089</v>
+        <v>3.400001199884355</v>
       </c>
       <c r="M6" t="n">
-        <v>4.734759217745054</v>
+        <v>5.472002700319376</v>
       </c>
       <c r="N6" t="n">
-        <v>4.798667812405541</v>
+        <v>5.756046004437871</v>
       </c>
       <c r="O6" t="n">
-        <v>3.914011340684613</v>
+        <v>4.465077789117872</v>
       </c>
       <c r="P6" t="n">
-        <v>3.262099164457679</v>
+        <v>2.860608106593312</v>
       </c>
       <c r="Q6" t="n">
-        <v>6.766020433767677</v>
+        <v>8.06971402011504</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Mean Noncovalent</t>
+          <t>Mean Isomerization</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9591900912914094</v>
+        <v>0.5554706594409674</v>
       </c>
       <c r="C7" t="n">
-        <v>1.453834932409892</v>
+        <v>1.30262562252924</v>
       </c>
       <c r="D7" t="n">
-        <v>1.025455264847285</v>
+        <v>1.22056851572857</v>
       </c>
       <c r="E7" t="n">
-        <v>2.373075812012285</v>
+        <v>1.903998258743017</v>
       </c>
       <c r="F7" t="n">
-        <v>2.740178413587454</v>
+        <v>3.066442516463451</v>
       </c>
       <c r="G7" t="n">
-        <v>2.386131006859464</v>
+        <v>1.761400181123495</v>
       </c>
       <c r="H7" t="n">
-        <v>2.150418035120464</v>
+        <v>1.608731078115534</v>
       </c>
       <c r="I7" t="n">
-        <v>3.145946171172196</v>
+        <v>1.594667840163088</v>
       </c>
       <c r="J7" t="n">
-        <v>3.60939403197893</v>
+        <v>1.76847405563724</v>
       </c>
       <c r="K7" t="n">
-        <v>3.948934948685842</v>
+        <v>2.762875133170416</v>
       </c>
       <c r="L7" t="n">
-        <v>4.869824980724623</v>
+        <v>3.012740638992309</v>
       </c>
       <c r="M7" t="n">
-        <v>4.758801721798166</v>
+        <v>3.435986542940126</v>
       </c>
       <c r="N7" t="n">
-        <v>5.13598360721227</v>
+        <v>3.603120007939581</v>
       </c>
       <c r="O7" t="n">
-        <v>7.373555411355149</v>
+        <v>3.252295269709014</v>
       </c>
       <c r="P7" t="n">
-        <v>8.769530284835964</v>
+        <v>2.340637216749883</v>
       </c>
       <c r="Q7" t="n">
-        <v>8.888967392803732</v>
+        <v>4.920660937042597</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Mean Thermochemistry</t>
+          <t>Mean Noncovalent</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.082773493478356</v>
+        <v>1.097451327629165</v>
       </c>
       <c r="C8" t="n">
-        <v>1.045558257542636</v>
+        <v>0.8907496469055344</v>
       </c>
       <c r="D8" t="n">
-        <v>1.54807296353547</v>
+        <v>1.408631313497661</v>
       </c>
       <c r="E8" t="n">
-        <v>1.586441936454559</v>
+        <v>0.9785908341633763</v>
       </c>
       <c r="F8" t="n">
-        <v>1.566750887927255</v>
+        <v>1.232059710847221</v>
       </c>
       <c r="G8" t="n">
-        <v>1.58935893435936</v>
+        <v>2.645796186753499</v>
       </c>
       <c r="H8" t="n">
-        <v>1.857097119963037</v>
+        <v>2.622894170617792</v>
       </c>
       <c r="I8" t="n">
-        <v>1.567773947503105</v>
+        <v>2.542658254902041</v>
       </c>
       <c r="J8" t="n">
-        <v>2.586671992343971</v>
+        <v>2.319516178483696</v>
       </c>
       <c r="K8" t="n">
-        <v>3.249400502616762</v>
+        <v>3.607798299111524</v>
       </c>
       <c r="L8" t="n">
-        <v>2.793076117120826</v>
+        <v>4.936263404742799</v>
       </c>
       <c r="M8" t="n">
-        <v>2.482367504616459</v>
+        <v>5.070317696035601</v>
       </c>
       <c r="N8" t="n">
-        <v>2.643610085214494</v>
+        <v>5.355664417772716</v>
       </c>
       <c r="O8" t="n">
-        <v>2.546895610970617</v>
+        <v>7.432988269066839</v>
       </c>
       <c r="P8" t="n">
-        <v>2.701696298740571</v>
+        <v>9.050913293739784</v>
       </c>
       <c r="Q8" t="n">
-        <v>3.894642972453799</v>
+        <v>9.16296128705798</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>Mean Thermochemistry</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.9246462968733978</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.109994036010521</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.05147331278402</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.567386731649206</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.653728971267002</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.463111649599972</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.578074208417043</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.571916769843446</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.78509715573366</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.525860194276377</v>
+      </c>
+      <c r="L9" t="n">
+        <v>2.621910765137486</v>
+      </c>
+      <c r="M9" t="n">
+        <v>2.353143933466784</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2.5051831055744</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2.391825476616795</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2.597332979979269</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>3.692115757406017</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>Mean Transition Metal</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>1.188965742659078</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.045936051186336</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.264929273877718</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2.280757777183448</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.743381216020994</v>
-      </c>
-      <c r="G9" t="n">
-        <v>2.22512839210896</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1.105911539787248</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.183620689743045</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1.649844704619394</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1.830891011363671</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1.360324636927957</v>
-      </c>
-      <c r="M9" t="n">
-        <v>1.605853918132687</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1.844879102605482</v>
-      </c>
-      <c r="O9" t="n">
-        <v>2.027249958665702</v>
-      </c>
-      <c r="P9" t="n">
-        <v>1.990592973912098</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>2.12018385176947</v>
+      <c r="B10" t="n">
+        <v>1.051872421684712</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.187662088716834</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.039248953079247</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.268111579774051</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.353032116155235</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.744404112116273</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.282591344538274</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2.222966651198293</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.103916968429391</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1.656858979878669</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.363581419509494</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.610199055411115</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.85042557165491</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2.034809750464644</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.989480660640204</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2.128674061919511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>